<commit_message>
dividindo pelo num de operaçoes
</commit_message>
<xml_diff>
--- a/etl/operacoes-credito/resources/fields-doc.xlsx
+++ b/etl/operacoes-credito/resources/fields-doc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
   <si>
     <t>codigo</t>
   </si>
@@ -160,9 +160,6 @@
     <t>origem</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>qt_numero_de_operacoes</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>m</t>
@@ -318,7 +318,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +329,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -371,7 +377,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -936,59 +942,53 @@
       <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="3" t="s">
         <v>58</v>
       </c>
       <c r="G14" s="1"/>
@@ -1145,9 +1145,7 @@
       <c r="F23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="G23" s="1"/>
       <c r="H23" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
@@ -1181,9 +1179,7 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
         <v>94</v>
       </c>
@@ -1201,9 +1197,7 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
refatorações na etl de operacoes-creditarias e documento de campos
</commit_message>
<xml_diff>
--- a/etl/operacoes-credito/resources/fields-doc.xlsx
+++ b/etl/operacoes-credito/resources/fields-doc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
   <si>
     <t>codigo</t>
   </si>
@@ -67,7 +67,7 @@
     <t>data_base</t>
   </si>
   <si>
-    <t>dt_data_base</t>
+    <t>dt_base</t>
   </si>
   <si>
     <t>d</t>
@@ -187,10 +187,7 @@
     <t>numero_de_operacoes</t>
   </si>
   <si>
-    <t>qt_numero_de_operacoes</t>
-  </si>
-  <si>
-    <t/>
+    <t>qt_operacoes</t>
   </si>
   <si>
     <t>m</t>
@@ -312,13 +309,19 @@
   <si>
     <t>Ativos Problemáticos - Carteira Inadimplida Arrastada</t>
   </si>
+  <si>
+    <t>Período (Ano)</t>
+  </si>
+  <si>
+    <t>dt_ano</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,12 +332,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -366,19 +363,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -694,17 +685,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="59.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="30.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="30.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="30.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="30.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="88.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="117.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="59.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="30.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="30.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="88.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="117.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -746,7 +737,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -762,7 +753,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -784,7 +775,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -806,7 +797,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -828,7 +819,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -850,7 +841,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -872,7 +863,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -894,7 +885,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -910,7 +901,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -932,7 +923,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -948,7 +939,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -972,7 +963,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -988,21 +979,19 @@
       <c r="E14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1010,15 +999,15 @@
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1026,15 +1015,15 @@
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1042,15 +1031,15 @@
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1058,15 +1047,15 @@
       <c r="G18" s="1"/>
       <c r="H18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1074,15 +1063,15 @@
       <c r="G19" s="1"/>
       <c r="H19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1090,15 +1079,15 @@
       <c r="G20" s="1"/>
       <c r="H20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1106,68 +1095,68 @@
       <c r="G21" s="1"/>
       <c r="H21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
@@ -1175,16 +1164,16 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -1193,26 +1182,32 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+      <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H26" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="2"/>
     </row>

</xml_diff>